<commit_message>
finished training goals B2 and activities planned B3
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\f32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C334C4-9028-4CC7-B5E6-77B0B8C02F12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72658E6-16DB-4485-8B53-09A6C360D53D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{C1A65C1F-CC53-4D23-B2FF-47F153ADAA5C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{C1A65C1F-CC53-4D23-B2FF-47F153ADAA5C}"/>
   </bookViews>
   <sheets>
     <sheet name="activities_planned" sheetId="1" r:id="rId1"/>
+    <sheet name="skills" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>Tasks</t>
   </si>
@@ -160,6 +161,87 @@
   </si>
   <si>
     <t>Total Training, Research, and Clinical Effort</t>
+  </si>
+  <si>
+    <t>F32 Training Plan</t>
+  </si>
+  <si>
+    <t>Core Skill</t>
+  </si>
+  <si>
+    <t>Competencies</t>
+  </si>
+  <si>
+    <t>Biostatistical and Computational Techniques</t>
+  </si>
+  <si>
+    <t>1. Coursework: EPI 538 and EPI 545</t>
+  </si>
+  <si>
+    <t>2. Coursework: ActiveEpi online training</t>
+  </si>
+  <si>
+    <t>3. Experiential Training: Research with Dr. Alonso and Dr. Vaccarino on study design</t>
+  </si>
+  <si>
+    <t>1. Coursework: BIOS 526, BIOS 534, and BIOS 731</t>
+  </si>
+  <si>
+    <t>3. Experiential Training: Statistical modeling of study variables, including linear and logistic regressions and survival analysis.</t>
+  </si>
+  <si>
+    <t>2. Experiential Training: ECG analysis with HRV Toolbox to strengthen understanding of raw data manipulation and time-series analysis with Dr. Shah</t>
+  </si>
+  <si>
+    <t>Neural Control of Cardiac Physiology</t>
+  </si>
+  <si>
+    <t>1. Coursework: Directed readings with Dr. Park on autonomic physiology.</t>
+  </si>
+  <si>
+    <t>2. Weekly lab and project meetings to understand clinical implications of ANS disease with Dr. Shah, Dr. Thames, and Dr. Park.</t>
+  </si>
+  <si>
+    <t>4. Improved manuscript and grant-writing skills</t>
+  </si>
+  <si>
+    <t>Epidemiology and Research Methods</t>
+  </si>
+  <si>
+    <t>5. Research presentation skills</t>
+  </si>
+  <si>
+    <t>3. Gain skills needed to understand and critically interpret epidemiological studies</t>
+  </si>
+  <si>
+    <t>2. Understand theory needed in the design of large cohort studies</t>
+  </si>
+  <si>
+    <t>1. Understand core concepts in epidemiology</t>
+  </si>
+  <si>
+    <t>1. Working knowledge of common statistical techniques</t>
+  </si>
+  <si>
+    <t>2. Ability to choose and perform increasingly complex statistically analyses with appropriate guidance</t>
+  </si>
+  <si>
+    <t>3. Become an informed collaborator in increasingly multidisciplinary computational methods</t>
+  </si>
+  <si>
+    <t>4. Increased understanding of MATLAB  and R software programming</t>
+  </si>
+  <si>
+    <t>1. Understanding content and foundational literature of autonomic physiology in relationship to neurocardiology</t>
+  </si>
+  <si>
+    <t>3. Mentoring and research meetings on psychological variables affect on heart with Dr. Vaccarino</t>
+  </si>
+  <si>
+    <t>2. Interpreting psychological epidemiology concepts, in particular qualitative assessments</t>
+  </si>
+  <si>
+    <t>1. Ability to create and interpret hypotheses from foundational, mechanism-oriented knowledge</t>
   </si>
 </sst>
 </file>
@@ -278,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -315,6 +397,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21431B15-486D-4B08-84E6-220E54DEBFE3}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -1074,4 +1159,132 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64DA9D3-7BEC-432C-B21C-739D282DE639}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C10" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>